<commit_message>
updated to do 64 samples each time
</commit_message>
<xml_diff>
--- a/ESP32_calibration/results.xlsx
+++ b/ESP32_calibration/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnp\code\AussieMeatCooker\ESP32_calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB22A0A1-1E2B-4BAB-A362-82C8CBA2B10E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECBFD244-CA48-4CC9-AEBB-BB90DD4FDB6F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18600" yWindow="1605" windowWidth="16605" windowHeight="12330" xr2:uid="{3D1116A1-E134-486E-9854-F4501D2E4775}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{3D1116A1-E134-486E-9854-F4501D2E4775}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
   <si>
     <t>adc []</t>
   </si>
@@ -48,22 +48,13 @@
     <t>Supply voltage</t>
   </si>
   <si>
-    <t>fluctuates 5 -&gt; 13</t>
-  </si>
-  <si>
     <t>Raw Input</t>
   </si>
   <si>
-    <t>Valid Range</t>
+    <t>Valid Range (200-2700 mv)</t>
   </si>
   <si>
-    <t>Input</t>
-  </si>
-  <si>
-    <t>Output</t>
-  </si>
-  <si>
-    <t>Testing</t>
+    <t>Valid Range (2700-3100 mv)</t>
   </si>
 </sst>
 </file>
@@ -95,27 +86,15 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -132,32 +111,16 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -233,407 +196,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>adc []</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="3"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="3175">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$B$5:$B$27</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="23"/>
-                <c:pt idx="3">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>140</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>190</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>200</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>520</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1050</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1729</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>2090</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>2380</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>2730</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>2990</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>3040</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>3100</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>3150</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>3180</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>3240</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$C$5:$C$27</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="23"/>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>68</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>460</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1106</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1560</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>2368</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>2737</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>3238</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>3750</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>3856</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>3997</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>4095</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>4095</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>4095</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-4B94-4D39-8D7A-D0311596A821}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="192658672"/>
-        <c:axId val="319772960"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="192658672"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="319772960"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="319772960"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="192658672"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$C$32</c:f>
+              <c:f>Sheet1!$C$38</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -674,11 +237,16 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="2"/>
+            <c:trendlineType val="linear"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.26763260013553342"/>
+                  <c:y val="-9.069881793911428E-3"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="#,##0.0000000000" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -711,78 +279,114 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$33:$B$42</c:f>
+              <c:f>Sheet1!$B$39:$B$54</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>80</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>460</c:v>
-                </c:pt>
                 <c:pt idx="2">
-                  <c:v>1106</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1982</c:v>
+                  <c:v>193</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2368</c:v>
+                  <c:v>436</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2738</c:v>
+                  <c:v>683</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3238</c:v>
+                  <c:v>916</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3750</c:v>
+                  <c:v>1164</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3856</c:v>
+                  <c:v>1409</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3945</c:v>
+                  <c:v>1650</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1889</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2130</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2377</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2625</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2877</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3159</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$33:$C$42</c:f>
+              <c:f>Sheet1!$C$39:$C$54</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>200</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>520</c:v>
-                </c:pt>
                 <c:pt idx="2">
-                  <c:v>1050</c:v>
+                  <c:v>250</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1770</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2090</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2390</c:v>
+                  <c:v>700</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2730</c:v>
+                  <c:v>900</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2990</c:v>
+                  <c:v>1100</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3040</c:v>
+                  <c:v>1300</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3080</c:v>
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1700</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1900</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2100</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2300</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2700</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -981,6 +585,943 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>actual (mV)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$5:$B$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>193</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>683</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>916</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1164</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1409</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1650</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1889</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2130</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2377</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2625</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2877</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3159</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3507</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3614</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3714</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3823</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$5:$C$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1700</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1900</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2100</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2300</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2700</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2900</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2950</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3050</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FEB8-4D79-AED1-FF01B04118E0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1301387135"/>
+        <c:axId val="1301381727"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1301387135"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>adc</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1301381727"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1301381727"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>V</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1301387135"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$62</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>actual (mV)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.14435673665791776"/>
+                  <c:y val="-5.0462962962962961E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="#,##0.0000000000" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$63:$B$70</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>3159</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3507</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3614</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3714</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3823</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3950</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4076</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$63:$C$70</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2700</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2900</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2950</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3050</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3150</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3476-436D-8D1B-E301E7FB7DC2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="111525488"/>
+        <c:axId val="111525904"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="111525488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="111525904"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="111525904"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="111525488"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1061,6 +1602,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2093,27 +2674,543 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1681</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>840</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>796564</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>187761</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>306481</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>65834</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>298174</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>182216</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8843678-8537-46CD-951F-DCE7AC330D6D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C836E3F-71B5-4505-A040-CF3AE9809416}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2133,23 +3230,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>465259</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>71804</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>339587</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>86140</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>172182</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>74735</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>8283</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>162340</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C836E3F-71B5-4505-A040-CF3AE9809416}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D28B25E-2A9F-4908-9EF8-EFDD8071FB93}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2162,6 +3259,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>70402</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>102704</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>352010</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>178904</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C040B9E4-FAFD-4684-A110-8CC3C37CF40D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2467,22 +3600,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2F98CF1-A2A6-4466-8C4C-E4AF1CDFD4B0}">
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.28515625" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.85546875" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -2490,346 +3624,574 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>3.24</v>
+        <v>3.28</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="B4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <f>D5</f>
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ref="C6:C31" si="0">D6</f>
+        <v>50</v>
+      </c>
+      <c r="D6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="D7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>18</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="D8">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>80</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="D9">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>135</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>250</v>
+      </c>
+      <c r="D10">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>193</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>300</v>
+      </c>
+      <c r="D11">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>436</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+      <c r="D12">
+        <f>D11+200</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>683</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>700</v>
+      </c>
+      <c r="D13">
+        <f t="shared" ref="D13:D24" si="1">D12+200</f>
+        <v>700</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>916</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>900</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="1"/>
+        <v>900</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>1164</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>1100</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="1"/>
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>1409</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>1300</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="1"/>
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>1650</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>1500</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="1"/>
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>1889</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>1700</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="1"/>
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>2130</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>1900</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="1"/>
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>2377</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>2100</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="1"/>
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>2625</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>2300</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="1"/>
+        <v>2300</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>2877</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>2500</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="1"/>
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>3159</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>2700</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="1"/>
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>3507</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>2900</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="1"/>
+        <v>2900</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>3614</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>2950</v>
+      </c>
+      <c r="D25">
+        <f t="shared" ref="D25:D31" si="2">D24+50</f>
+        <v>2950</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>3714</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>3000</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="2"/>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>3823</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>3050</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="2"/>
+        <v>3050</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>3950</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>3100</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="2"/>
+        <v>3100</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>4076</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>3150</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="2"/>
+        <v>3150</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>4095</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>3200</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="2"/>
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>4095</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>3250</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="2"/>
+        <v>3250</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="1" t="s">
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>18</v>
+      </c>
+      <c r="C39">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>80</v>
+      </c>
+      <c r="C40">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <v>135</v>
+      </c>
+      <c r="C41">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>193</v>
+      </c>
+      <c r="C42">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>436</v>
+      </c>
+      <c r="C43">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <v>683</v>
+      </c>
+      <c r="C44">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B45">
+        <v>916</v>
+      </c>
+      <c r="C45">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B46">
+        <v>1164</v>
+      </c>
+      <c r="C46">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B47">
+        <v>1409</v>
+      </c>
+      <c r="C47">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B48">
+        <v>1650</v>
+      </c>
+      <c r="C48">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B49">
+        <v>1889</v>
+      </c>
+      <c r="C49">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B50">
+        <v>2130</v>
+      </c>
+      <c r="C50">
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B51">
+        <v>2377</v>
+      </c>
+      <c r="C51">
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B52">
+        <v>2625</v>
+      </c>
+      <c r="C52">
+        <v>2300</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B53">
+        <v>2877</v>
+      </c>
+      <c r="C53">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B54">
+        <v>3159</v>
+      </c>
+      <c r="C54">
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B62" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>75</v>
-      </c>
-      <c r="B8">
-        <v>70</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>100</v>
-      </c>
-      <c r="B9">
-        <v>100</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>150</v>
-      </c>
-      <c r="B11">
-        <v>140</v>
-      </c>
-      <c r="C11">
-        <v>10</v>
-      </c>
-      <c r="D11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>175</v>
-      </c>
-      <c r="B12">
-        <v>190</v>
-      </c>
-      <c r="C12">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>200</v>
-      </c>
-      <c r="B13">
-        <v>200</v>
-      </c>
-      <c r="C13">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>400</v>
-      </c>
-      <c r="B14">
-        <v>520</v>
-      </c>
-      <c r="C14">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>1000</v>
-      </c>
-      <c r="B16">
-        <v>1050</v>
-      </c>
-      <c r="C16">
-        <v>1106</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>1300</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>1600</v>
-      </c>
-      <c r="B18">
-        <v>1729</v>
-      </c>
-      <c r="C18">
-        <v>1560</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>1900</v>
-      </c>
-      <c r="B19">
-        <v>2090</v>
-      </c>
-      <c r="C19">
-        <v>2368</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>2200</v>
-      </c>
-      <c r="B20">
-        <v>2380</v>
-      </c>
-      <c r="C20">
-        <v>2737</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>2500</v>
-      </c>
-      <c r="B21">
-        <v>2730</v>
-      </c>
-      <c r="C21">
-        <v>3238</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>2800</v>
-      </c>
-      <c r="B22">
-        <v>2990</v>
-      </c>
-      <c r="C22">
-        <v>3750</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B23">
-        <v>3040</v>
-      </c>
-      <c r="C23">
-        <v>3856</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B24">
+      <c r="C62" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B63">
+        <v>3159</v>
+      </c>
+      <c r="C63">
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B64">
+        <v>3507</v>
+      </c>
+      <c r="C64">
+        <v>2900</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B65">
+        <v>3614</v>
+      </c>
+      <c r="C65">
+        <v>2950</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B66">
+        <v>3714</v>
+      </c>
+      <c r="C66">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B67">
+        <v>3823</v>
+      </c>
+      <c r="C67">
+        <v>3050</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B68">
+        <v>3950</v>
+      </c>
+      <c r="C68">
         <v>3100</v>
       </c>
-      <c r="C24">
-        <v>3997</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B25">
+    </row>
+    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B69">
+        <v>4076</v>
+      </c>
+      <c r="C69">
         <v>3150</v>
-      </c>
-      <c r="C25">
-        <v>4095</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>3100</v>
-      </c>
-      <c r="B26">
-        <v>3180</v>
-      </c>
-      <c r="C26">
-        <v>4095</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>3400</v>
-      </c>
-      <c r="B27">
-        <v>3240</v>
-      </c>
-      <c r="C27">
-        <v>4095</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B32" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B33">
-        <v>80</v>
-      </c>
-      <c r="C33">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B34">
-        <v>460</v>
-      </c>
-      <c r="C34">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B35">
-        <v>1106</v>
-      </c>
-      <c r="C35">
-        <v>1050</v>
-      </c>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B36">
-        <v>1982</v>
-      </c>
-      <c r="C36">
-        <v>1770</v>
-      </c>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B37">
-        <v>2368</v>
-      </c>
-      <c r="C37">
-        <v>2090</v>
-      </c>
-    </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B38">
-        <v>2738</v>
-      </c>
-      <c r="C38">
-        <v>2390</v>
-      </c>
-    </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B39">
-        <v>3238</v>
-      </c>
-      <c r="C39">
-        <v>2730</v>
-      </c>
-    </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B40">
-        <v>3750</v>
-      </c>
-      <c r="C40">
-        <v>2990</v>
-      </c>
-    </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B41">
-        <v>3856</v>
-      </c>
-      <c r="C41">
-        <v>3040</v>
-      </c>
-    </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B42">
-        <v>3945</v>
-      </c>
-      <c r="C42">
-        <v>3080</v>
-      </c>
-    </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B44" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C44" s="3"/>
-    </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B45" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B46" s="4">
-        <v>2485</v>
-      </c>
-      <c r="C46" s="6">
-        <f>(0.0000495665*B46^2 + 0.9590164706*B46 + 94.1840600468)/1000</f>
-        <v>2.7834242794502999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed issue cutting down range
</commit_message>
<xml_diff>
--- a/ESP32_calibration/results.xlsx
+++ b/ESP32_calibration/results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnp\code\AussieMeatCooker\ESP32_calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECBFD244-CA48-4CC9-AEBB-BB90DD4FDB6F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7FA08C5-1430-4316-9199-03F472D4EB26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{3D1116A1-E134-486E-9854-F4501D2E4775}"/>
+    <workbookView xWindow="7635" yWindow="240" windowWidth="25695" windowHeight="11385" xr2:uid="{3D1116A1-E134-486E-9854-F4501D2E4775}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3600,10 +3600,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2F98CF1-A2A6-4466-8C4C-E4AF1CDFD4B0}">
-  <dimension ref="A1:D69"/>
+  <dimension ref="A1:O69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3982,13 +3982,13 @@
         <v>3250</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:15" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
         <v>0</v>
       </c>
@@ -3996,7 +3996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B39">
         <v>18</v>
       </c>
@@ -4004,7 +4004,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B40">
         <v>80</v>
       </c>
@@ -4012,7 +4012,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B41">
         <v>135</v>
       </c>
@@ -4020,7 +4020,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B42">
         <v>193</v>
       </c>
@@ -4028,7 +4028,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B43">
         <v>436</v>
       </c>
@@ -4036,15 +4036,19 @@
         <v>500</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B44">
         <v>683</v>
       </c>
       <c r="C44">
         <v>700</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="O44">
+        <f>0.8194542611*20 + 142.7653067728</f>
+        <v>159.15439199479999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B45">
         <v>916</v>
       </c>
@@ -4052,7 +4056,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B46">
         <v>1164</v>
       </c>
@@ -4060,7 +4064,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B47">
         <v>1409</v>
       </c>
@@ -4068,7 +4072,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B48">
         <v>1650</v>
       </c>

</xml_diff>